<commit_message>
too much stuff to list
</commit_message>
<xml_diff>
--- a/ExcelAssessmentIntegration/ExcelAssessmentIntegration/bin/dataSheets/17_summer_CPSC246_2.xlsx
+++ b/ExcelAssessmentIntegration/ExcelAssessmentIntegration/bin/dataSheets/17_summer_CPSC246_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\College Work\ExcelAssessmentIntegration\CPSC236FinalProject\ExcelAssessmentIntegration\ExcelAssessmentIntegration\bin\dataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86C2003-2FE6-4BC0-9F6B-8E8B1387A4A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E292F9-69A7-44DB-8DA2-7AE7676041E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{267C837C-C0E8-4FFE-8F95-51316AE109C3}"/>
   </bookViews>
@@ -33,23 +33,29 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>example objective 1</t>
+    <t>obj1</t>
   </si>
   <si>
-    <t>example objective 4</t>
+    <t>obj2</t>
   </si>
   <si>
-    <t>example objective 12</t>
+    <t>obj3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -394,7 +400,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +424,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>14</v>
@@ -432,7 +438,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>65</v>
@@ -445,6 +451,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>